<commit_message>
Fixed substrate volcanos for good.
</commit_message>
<xml_diff>
--- a/test_files/cyclopropanation.xlsx
+++ b/test_files/cyclopropanation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -49,31 +49,10 @@
     <t xml:space="preserve">TS(P4,1)</t>
   </si>
   <si>
-    <t xml:space="preserve">TS(A4,A5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS(A5,A6)-CN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS(A5,A6)-CC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS(1,A2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">P</t>
   </si>
   <si>
     <t xml:space="preserve">Co-Ligand1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">–62.54</t>
   </si>
   <si>
     <t xml:space="preserve">Co-Ligand2</t>
@@ -203,9 +182,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -300,7 +280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -315,6 +295,10 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -334,13 +318,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:P43"/>
+      <selection pane="topLeft" activeCell="M32" activeCellId="0" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -370,31 +354,13 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>0</v>
@@ -420,31 +386,13 @@
       <c r="I2" s="3" t="n">
         <v>4.6</v>
       </c>
-      <c r="J2" s="3" t="n">
-        <v>5.18</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>3.43</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>17.27</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>-46.19</v>
-      </c>
-      <c r="N2" s="3" t="n">
-        <v>18.51</v>
-      </c>
-      <c r="O2" s="3" t="n">
-        <v>31.9</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>17</v>
+      <c r="J2" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>0</v>
@@ -470,31 +418,13 @@
       <c r="I3" s="3" t="n">
         <v>14.79</v>
       </c>
-      <c r="J3" s="3" t="n">
-        <v>16.44</v>
-      </c>
-      <c r="K3" s="3" t="n">
-        <v>9.3</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>13.83</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>-52.67</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>25.43</v>
-      </c>
-      <c r="O3" s="3" t="n">
-        <v>31.59</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>17</v>
+      <c r="J3" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0</v>
@@ -520,31 +450,13 @@
       <c r="I4" s="3" t="n">
         <v>23.69</v>
       </c>
-      <c r="J4" s="3" t="n">
-        <v>18.63</v>
-      </c>
-      <c r="K4" s="3" t="n">
-        <v>14.52</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>16.66</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>-48.57</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>29</v>
-      </c>
-      <c r="O4" s="3" t="n">
-        <v>29.92</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>17</v>
+      <c r="J4" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>0</v>
@@ -570,31 +482,13 @@
       <c r="I5" s="3" t="n">
         <v>23.66</v>
       </c>
-      <c r="J5" s="3" t="n">
-        <v>19.16</v>
-      </c>
-      <c r="K5" s="3" t="n">
-        <v>11.13</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>-49.48</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>21.14</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>31.87</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>17</v>
+      <c r="J5" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0</v>
@@ -620,31 +514,13 @@
       <c r="I6" s="3" t="n">
         <v>25.18</v>
       </c>
-      <c r="J6" s="3" t="n">
-        <v>17.46</v>
-      </c>
-      <c r="K6" s="3" t="n">
-        <v>11.8</v>
-      </c>
-      <c r="L6" s="3" t="n">
-        <v>17.89</v>
-      </c>
-      <c r="M6" s="3" t="n">
-        <v>-42.92</v>
-      </c>
-      <c r="N6" s="3" t="n">
-        <v>23.3</v>
-      </c>
-      <c r="O6" s="3" t="n">
-        <v>30.97</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>17</v>
+      <c r="J6" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0</v>
@@ -670,31 +546,13 @@
       <c r="I7" s="3" t="n">
         <v>14.05</v>
       </c>
-      <c r="J7" s="3" t="n">
-        <v>18.08</v>
-      </c>
-      <c r="K7" s="3" t="n">
-        <v>13.44</v>
-      </c>
-      <c r="L7" s="3" t="n">
-        <v>18.44</v>
-      </c>
-      <c r="M7" s="3" t="n">
-        <v>-36.2</v>
-      </c>
-      <c r="N7" s="3" t="n">
-        <v>26.1</v>
-      </c>
-      <c r="O7" s="3" t="n">
-        <v>32.55</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>17</v>
+      <c r="J7" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>0</v>
@@ -720,31 +578,13 @@
       <c r="I8" s="3" t="n">
         <v>7.77</v>
       </c>
-      <c r="J8" s="3" t="n">
-        <v>14.22</v>
-      </c>
-      <c r="K8" s="3" t="n">
-        <v>7.95</v>
-      </c>
-      <c r="L8" s="3" t="n">
-        <v>27.15</v>
-      </c>
-      <c r="M8" s="3" t="n">
-        <v>-52.77</v>
-      </c>
-      <c r="N8" s="3" t="n">
-        <v>23.17</v>
-      </c>
-      <c r="O8" s="3" t="n">
-        <v>33.72</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>17</v>
+      <c r="J8" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>0</v>
@@ -770,31 +610,13 @@
       <c r="I9" s="3" t="n">
         <v>15.9</v>
       </c>
-      <c r="J9" s="3" t="n">
-        <v>10.05</v>
-      </c>
-      <c r="K9" s="3" t="n">
-        <v>5.68</v>
-      </c>
-      <c r="L9" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="M9" s="3" t="n">
-        <v>-52.05</v>
-      </c>
-      <c r="N9" s="3" t="n">
-        <v>9.31</v>
-      </c>
-      <c r="O9" s="3" t="n">
-        <v>31.66</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>17</v>
+      <c r="J9" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>0</v>
@@ -820,31 +642,13 @@
       <c r="I10" s="3" t="n">
         <v>17.69</v>
       </c>
-      <c r="J10" s="3" t="n">
-        <v>16.11</v>
-      </c>
-      <c r="K10" s="3" t="n">
-        <v>11.13</v>
-      </c>
-      <c r="L10" s="3" t="n">
-        <v>15.69</v>
-      </c>
-      <c r="M10" s="3" t="n">
-        <v>-45.27</v>
-      </c>
-      <c r="N10" s="3" t="n">
-        <v>28.44</v>
-      </c>
-      <c r="O10" s="3" t="n">
-        <v>31.41</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>17</v>
+      <c r="J10" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>0</v>
@@ -870,31 +674,13 @@
       <c r="I11" s="3" t="n">
         <v>26.33</v>
       </c>
-      <c r="J11" s="3" t="n">
-        <v>10.45</v>
-      </c>
-      <c r="K11" s="3" t="n">
-        <v>3.54</v>
-      </c>
-      <c r="L11" s="3" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>-50.04</v>
-      </c>
-      <c r="N11" s="3" t="n">
-        <v>20.89</v>
-      </c>
-      <c r="O11" s="3" t="n">
-        <v>34.5</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>17</v>
+      <c r="J11" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>0</v>
@@ -920,31 +706,13 @@
       <c r="I12" s="3" t="n">
         <v>27.01</v>
       </c>
-      <c r="J12" s="3" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="K12" s="3" t="n">
-        <v>9.07</v>
-      </c>
-      <c r="L12" s="3" t="n">
-        <v>21.8</v>
-      </c>
-      <c r="M12" s="3" t="n">
-        <v>-38.34</v>
-      </c>
-      <c r="N12" s="3" t="n">
-        <v>25.31</v>
-      </c>
-      <c r="O12" s="3" t="n">
-        <v>29.61</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>17</v>
+      <c r="J12" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>0</v>
@@ -970,31 +738,13 @@
       <c r="I13" s="3" t="n">
         <v>22.51</v>
       </c>
-      <c r="J13" s="3" t="n">
-        <v>16.06</v>
-      </c>
-      <c r="K13" s="3" t="n">
-        <v>12.88</v>
-      </c>
-      <c r="L13" s="3" t="n">
-        <v>19.67</v>
-      </c>
-      <c r="M13" s="3" t="n">
-        <v>-42.19</v>
-      </c>
-      <c r="N13" s="3" t="n">
-        <v>27.22</v>
-      </c>
-      <c r="O13" s="3" t="n">
-        <v>31.74</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>17</v>
+      <c r="J13" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>0</v>
@@ -1020,31 +770,13 @@
       <c r="I14" s="3" t="n">
         <v>22.5</v>
       </c>
-      <c r="J14" s="3" t="n">
-        <v>19.95</v>
-      </c>
-      <c r="K14" s="3" t="n">
-        <v>12.76</v>
-      </c>
-      <c r="L14" s="3" t="n">
-        <v>29.98</v>
-      </c>
-      <c r="M14" s="3" t="n">
-        <v>-44.97</v>
-      </c>
-      <c r="N14" s="3" t="n">
-        <v>23.44</v>
-      </c>
-      <c r="O14" s="3" t="n">
-        <v>32.83</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>17</v>
+      <c r="J14" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>0</v>
@@ -1070,31 +802,13 @@
       <c r="I15" s="3" t="n">
         <v>19.7</v>
       </c>
-      <c r="J15" s="3" t="n">
-        <v>15.92</v>
-      </c>
-      <c r="K15" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="L15" s="3" t="n">
-        <v>20.07</v>
-      </c>
-      <c r="M15" s="3" t="n">
-        <v>-49.21</v>
-      </c>
-      <c r="N15" s="3" t="n">
-        <v>29.02</v>
-      </c>
-      <c r="O15" s="3" t="n">
-        <v>31.1</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>17</v>
+      <c r="J15" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>0</v>
@@ -1120,31 +834,13 @@
       <c r="I16" s="3" t="n">
         <v>-10.79</v>
       </c>
-      <c r="J16" s="3" t="n">
-        <v>-1.69</v>
-      </c>
-      <c r="K16" s="3" t="n">
-        <v>-5.55</v>
-      </c>
-      <c r="L16" s="3" t="n">
-        <v>11.69</v>
-      </c>
-      <c r="M16" s="3" t="n">
-        <v>-55.26</v>
-      </c>
-      <c r="N16" s="3" t="n">
-        <v>14.11</v>
-      </c>
-      <c r="O16" s="3" t="n">
-        <v>28.59</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>17</v>
+      <c r="J16" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>0</v>
@@ -1170,31 +866,13 @@
       <c r="I17" s="3" t="n">
         <v>-2.03</v>
       </c>
-      <c r="J17" s="3" t="n">
-        <v>13.16</v>
-      </c>
-      <c r="K17" s="3" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="L17" s="3" t="n">
-        <v>12.93</v>
-      </c>
-      <c r="M17" s="3" t="n">
-        <v>-52.82</v>
-      </c>
-      <c r="N17" s="3" t="n">
-        <v>24.78</v>
-      </c>
-      <c r="O17" s="3" t="n">
-        <v>29.51</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>17</v>
+      <c r="J17" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>0</v>
@@ -1220,31 +898,13 @@
       <c r="I18" s="3" t="n">
         <v>5.22</v>
       </c>
-      <c r="J18" s="3" t="n">
-        <v>10.81</v>
-      </c>
-      <c r="K18" s="3" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="L18" s="3" t="n">
-        <v>11.36</v>
-      </c>
-      <c r="M18" s="3" t="n">
-        <v>-45.88</v>
-      </c>
-      <c r="N18" s="3" t="n">
-        <v>23.31</v>
-      </c>
-      <c r="O18" s="3" t="n">
-        <v>26.98</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>17</v>
+      <c r="J18" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>0</v>
@@ -1270,31 +930,13 @@
       <c r="I19" s="3" t="n">
         <v>7.71</v>
       </c>
-      <c r="J19" s="3" t="n">
-        <v>11.92</v>
-      </c>
-      <c r="K19" s="3" t="n">
-        <v>5.74</v>
-      </c>
-      <c r="L19" s="3" t="n">
-        <v>9.91</v>
-      </c>
-      <c r="M19" s="3" t="n">
-        <v>-52.17</v>
-      </c>
-      <c r="N19" s="3" t="n">
-        <v>13.86</v>
-      </c>
-      <c r="O19" s="3" t="n">
-        <v>30.59</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>17</v>
+      <c r="J19" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>0</v>
@@ -1320,31 +962,13 @@
       <c r="I20" s="3" t="n">
         <v>2.7</v>
       </c>
-      <c r="J20" s="3" t="n">
-        <v>7.59</v>
-      </c>
-      <c r="K20" s="3" t="n">
-        <v>3.91</v>
-      </c>
-      <c r="L20" s="3" t="n">
-        <v>17.74</v>
-      </c>
-      <c r="M20" s="3" t="n">
-        <v>-49.27</v>
-      </c>
-      <c r="N20" s="3" t="n">
-        <v>12.55</v>
-      </c>
-      <c r="O20" s="3" t="n">
-        <v>28.61</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>17</v>
+      <c r="J20" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>0</v>
@@ -1370,31 +994,13 @@
       <c r="I21" s="3" t="n">
         <v>-4.64</v>
       </c>
-      <c r="J21" s="3" t="n">
-        <v>9.94</v>
-      </c>
-      <c r="K21" s="3" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="L21" s="3" t="n">
-        <v>11.24</v>
-      </c>
-      <c r="M21" s="3" t="n">
-        <v>-47.83</v>
-      </c>
-      <c r="N21" s="3" t="n">
-        <v>19.93</v>
-      </c>
-      <c r="O21" s="3" t="n">
-        <v>30.87</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>17</v>
+      <c r="J21" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>0</v>
@@ -1420,31 +1026,13 @@
       <c r="I22" s="3" t="n">
         <v>-8.39</v>
       </c>
-      <c r="J22" s="3" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="K22" s="3" t="n">
-        <v>-2.75</v>
-      </c>
-      <c r="L22" s="3" t="n">
-        <v>21.52</v>
-      </c>
-      <c r="M22" s="3" t="n">
-        <v>-58.14</v>
-      </c>
-      <c r="N22" s="3" t="n">
-        <v>17.78</v>
-      </c>
-      <c r="O22" s="3" t="n">
-        <v>28.57</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>17</v>
+      <c r="J22" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>0</v>
@@ -1470,31 +1058,13 @@
       <c r="I23" s="3" t="n">
         <v>0.49</v>
       </c>
-      <c r="J23" s="3" t="n">
-        <v>1.26</v>
-      </c>
-      <c r="K23" s="3" t="n">
-        <v>-3.18</v>
-      </c>
-      <c r="L23" s="3" t="n">
-        <v>8.68</v>
-      </c>
-      <c r="M23" s="3" t="n">
-        <v>-57.94</v>
-      </c>
-      <c r="N23" s="3" t="n">
-        <v>7.91</v>
-      </c>
-      <c r="O23" s="3" t="n">
-        <v>29.57</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>17</v>
+      <c r="J23" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>0</v>
@@ -1520,31 +1090,13 @@
       <c r="I24" s="3" t="n">
         <v>-0.18</v>
       </c>
-      <c r="J24" s="3" t="n">
-        <v>11.11</v>
-      </c>
-      <c r="K24" s="3" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="L24" s="3" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="M24" s="3" t="n">
-        <v>-52.56</v>
-      </c>
-      <c r="N24" s="3" t="n">
-        <v>25.1</v>
-      </c>
-      <c r="O24" s="3" t="n">
-        <v>30.74</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>17</v>
+      <c r="J24" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>0</v>
@@ -1570,31 +1122,13 @@
       <c r="I25" s="3" t="n">
         <v>8.04</v>
       </c>
-      <c r="J25" s="3" t="n">
-        <v>3.99</v>
-      </c>
-      <c r="K25" s="3" t="n">
-        <v>-6.8</v>
-      </c>
-      <c r="L25" s="3" t="n">
-        <v>9.55</v>
-      </c>
-      <c r="M25" s="3" t="n">
-        <v>-57.09</v>
-      </c>
-      <c r="N25" s="3" t="n">
-        <v>14.64</v>
-      </c>
-      <c r="O25" s="3" t="n">
-        <v>32.19</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>17</v>
+      <c r="J25" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>0</v>
@@ -1620,31 +1154,13 @@
       <c r="I26" s="3" t="n">
         <v>3.08</v>
       </c>
-      <c r="J26" s="3" t="n">
-        <v>5.11</v>
-      </c>
-      <c r="K26" s="3" t="n">
-        <v>-2.02</v>
-      </c>
-      <c r="L26" s="3" t="n">
-        <v>12.52</v>
-      </c>
-      <c r="M26" s="3" t="n">
-        <v>-51.24</v>
-      </c>
-      <c r="N26" s="3" t="n">
-        <v>18.59</v>
-      </c>
-      <c r="O26" s="3" t="n">
-        <v>27.11</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>17</v>
+      <c r="J26" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>0</v>
@@ -1670,31 +1186,13 @@
       <c r="I27" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="J27" s="3" t="n">
-        <v>8.96</v>
-      </c>
-      <c r="K27" s="3" t="n">
-        <v>2.56</v>
-      </c>
-      <c r="L27" s="3" t="n">
-        <v>15.13</v>
-      </c>
-      <c r="M27" s="3" t="n">
-        <v>-50.95</v>
-      </c>
-      <c r="N27" s="3" t="n">
-        <v>23.14</v>
-      </c>
-      <c r="O27" s="3" t="n">
-        <v>30.05</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>17</v>
+      <c r="J27" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>0</v>
@@ -1720,31 +1218,13 @@
       <c r="I28" s="3" t="n">
         <v>-5.58</v>
       </c>
-      <c r="J28" s="3" t="n">
-        <v>6.22</v>
-      </c>
-      <c r="K28" s="3" t="n">
-        <v>-0.33</v>
-      </c>
-      <c r="L28" s="3" t="n">
-        <v>18.34</v>
-      </c>
-      <c r="M28" s="3" t="n">
-        <v>-55.21</v>
-      </c>
-      <c r="N28" s="3" t="n">
-        <v>13.68</v>
-      </c>
-      <c r="O28" s="3" t="n">
-        <v>27.49</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>17</v>
+      <c r="J28" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>0</v>
@@ -1770,31 +1250,13 @@
       <c r="I29" s="3" t="n">
         <v>-1.3</v>
       </c>
-      <c r="J29" s="3" t="n">
-        <v>12.03</v>
-      </c>
-      <c r="K29" s="3" t="n">
-        <v>3.99</v>
-      </c>
-      <c r="L29" s="3" t="n">
-        <v>17.09</v>
-      </c>
-      <c r="M29" s="3" t="n">
-        <v>-51.39</v>
-      </c>
-      <c r="N29" s="3" t="n">
-        <v>24.88</v>
-      </c>
-      <c r="O29" s="3" t="n">
-        <v>29.92</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>17</v>
+      <c r="J29" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>0</v>
@@ -1820,31 +1282,13 @@
       <c r="I30" s="3" t="n">
         <v>-21.17</v>
       </c>
-      <c r="J30" s="3" t="n">
-        <v>-10.03</v>
-      </c>
-      <c r="K30" s="3" t="n">
-        <v>-21.24</v>
-      </c>
-      <c r="L30" s="3" t="n">
-        <v>3.24</v>
-      </c>
-      <c r="M30" s="3" t="n">
-        <v>-55.83</v>
-      </c>
-      <c r="N30" s="3" t="n">
-        <v>11.84</v>
-      </c>
-      <c r="O30" s="3" t="n">
-        <v>26.73</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>17</v>
+      <c r="J30" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>0</v>
@@ -1870,31 +1314,13 @@
       <c r="I31" s="3" t="n">
         <v>-11.15</v>
       </c>
-      <c r="J31" s="3" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="K31" s="3" t="n">
-        <v>-15.29</v>
-      </c>
-      <c r="L31" s="3" t="n">
-        <v>-1.37</v>
-      </c>
-      <c r="M31" s="3" t="n">
-        <v>-55.54</v>
-      </c>
-      <c r="N31" s="3" t="n">
-        <v>17.43</v>
-      </c>
-      <c r="O31" s="3" t="n">
-        <v>27.07</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>17</v>
+      <c r="J31" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>0</v>
@@ -1920,31 +1346,13 @@
       <c r="I32" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="J32" s="3" t="n">
-        <v>1.64</v>
-      </c>
-      <c r="K32" s="3" t="n">
-        <v>-11.42</v>
-      </c>
-      <c r="L32" s="3" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="M32" s="3" t="n">
-        <v>-52.98</v>
-      </c>
-      <c r="N32" s="3" t="n">
-        <v>18.91</v>
-      </c>
-      <c r="O32" s="3" t="n">
-        <v>25.8</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>17</v>
+      <c r="J32" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>0</v>
@@ -1970,31 +1378,13 @@
       <c r="I33" s="3" t="n">
         <v>2.43</v>
       </c>
-      <c r="J33" s="3" t="n">
-        <v>-0.23</v>
-      </c>
-      <c r="K33" s="3" t="n">
-        <v>-13.75</v>
-      </c>
-      <c r="L33" s="3" t="n">
-        <v>-3.51</v>
-      </c>
-      <c r="M33" s="3" t="n">
-        <v>-58.18</v>
-      </c>
-      <c r="N33" s="3" t="n">
-        <v>2.21</v>
-      </c>
-      <c r="O33" s="3" t="n">
-        <v>27.55</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>17</v>
+      <c r="J33" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>0</v>
@@ -2020,31 +1410,13 @@
       <c r="I34" s="3" t="n">
         <v>-4.08</v>
       </c>
-      <c r="J34" s="3" t="n">
-        <v>-1.44</v>
-      </c>
-      <c r="K34" s="3" t="n">
-        <v>-13.32</v>
-      </c>
-      <c r="L34" s="3" t="n">
-        <v>5.68</v>
-      </c>
-      <c r="M34" s="3" t="n">
-        <v>-58.13</v>
-      </c>
-      <c r="N34" s="3" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="O34" s="3" t="n">
-        <v>26.21</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>17</v>
+      <c r="J34" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>0</v>
@@ -2070,31 +1442,13 @@
       <c r="I35" s="3" t="n">
         <v>-12.03</v>
       </c>
-      <c r="J35" s="3" t="n">
-        <v>-3.77</v>
-      </c>
-      <c r="K35" s="3" t="n">
-        <v>-17.29</v>
-      </c>
-      <c r="L35" s="3" t="n">
-        <v>-1.68</v>
-      </c>
-      <c r="M35" s="3" t="n">
-        <v>-54.46</v>
-      </c>
-      <c r="N35" s="3" t="n">
-        <v>13.02</v>
-      </c>
-      <c r="O35" s="3" t="n">
-        <v>29.14</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>17</v>
+      <c r="J35" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>0</v>
@@ -2120,31 +1474,13 @@
       <c r="I36" s="3" t="n">
         <v>-17.78</v>
       </c>
-      <c r="J36" s="3" t="n">
-        <v>-5.03</v>
-      </c>
-      <c r="K36" s="3" t="n">
-        <v>-18.63</v>
-      </c>
-      <c r="L36" s="3" t="n">
-        <v>12.54</v>
-      </c>
-      <c r="M36" s="3" t="n">
-        <v>-62.28</v>
-      </c>
-      <c r="N36" s="3" t="n">
-        <v>12.31</v>
-      </c>
-      <c r="O36" s="3" t="n">
-        <v>27.98</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>17</v>
+      <c r="J36" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>0</v>
@@ -2170,31 +1506,13 @@
       <c r="I37" s="3" t="n">
         <v>-4.95</v>
       </c>
-      <c r="J37" s="3" t="n">
-        <v>-6.75</v>
-      </c>
-      <c r="K37" s="3" t="n">
-        <v>-17.74</v>
-      </c>
-      <c r="L37" s="3" t="n">
-        <v>-3.92</v>
-      </c>
-      <c r="M37" s="3" t="n">
-        <v>-63.34</v>
-      </c>
-      <c r="N37" s="3" t="n">
-        <v>3.86</v>
-      </c>
-      <c r="O37" s="3" t="n">
-        <v>27.92</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>17</v>
+      <c r="J37" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>0</v>
@@ -2220,31 +1538,13 @@
       <c r="I38" s="3" t="n">
         <v>-8.34</v>
       </c>
-      <c r="J38" s="3" t="n">
-        <v>1.58</v>
-      </c>
-      <c r="K38" s="3" t="n">
-        <v>-12.94</v>
-      </c>
-      <c r="L38" s="3" t="n">
-        <v>2.43</v>
-      </c>
-      <c r="M38" s="3" t="n">
-        <v>-60.32</v>
-      </c>
-      <c r="N38" s="3" t="n">
-        <v>19.86</v>
-      </c>
-      <c r="O38" s="3" t="n">
-        <v>28.08</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>17</v>
+      <c r="J38" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>0</v>
@@ -2270,31 +1570,13 @@
       <c r="I39" s="3" t="n">
         <v>-0.06</v>
       </c>
-      <c r="J39" s="3" t="n">
-        <v>-6.96</v>
-      </c>
-      <c r="K39" s="3" t="n">
-        <v>-22.34</v>
-      </c>
-      <c r="L39" s="3" t="n">
-        <v>-1.88</v>
-      </c>
-      <c r="M39" s="3" t="n">
-        <v>-61.74</v>
-      </c>
-      <c r="N39" s="3" t="n">
-        <v>10.6</v>
-      </c>
-      <c r="O39" s="3" t="n">
-        <v>29.09</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>17</v>
+      <c r="J39" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>0</v>
@@ -2320,31 +1602,13 @@
       <c r="I40" s="3" t="n">
         <v>-2.6</v>
       </c>
-      <c r="J40" s="3" t="n">
-        <v>-3.37</v>
-      </c>
-      <c r="K40" s="3" t="n">
-        <v>-15.54</v>
-      </c>
-      <c r="L40" s="3" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="M40" s="3" t="n">
-        <v>-56.13</v>
-      </c>
-      <c r="N40" s="3" t="n">
-        <v>16.69</v>
-      </c>
-      <c r="O40" s="3" t="n">
-        <v>26.26</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>17</v>
+      <c r="J40" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>0</v>
@@ -2370,31 +1634,13 @@
       <c r="I41" s="3" t="n">
         <v>-8.2</v>
       </c>
-      <c r="J41" s="3" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="K41" s="3" t="n">
-        <v>-12.55</v>
-      </c>
-      <c r="L41" s="3" t="n">
-        <v>4.78</v>
-      </c>
-      <c r="M41" s="3" t="n">
-        <v>-57.5</v>
-      </c>
-      <c r="N41" s="3" t="n">
-        <v>18.3</v>
-      </c>
-      <c r="O41" s="3" t="n">
-        <v>27.56</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>17</v>
+      <c r="J41" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>0</v>
@@ -2420,31 +1666,13 @@
       <c r="I42" s="3" t="n">
         <v>-12.11</v>
       </c>
-      <c r="J42" s="3" t="n">
-        <v>-3.2</v>
-      </c>
-      <c r="K42" s="3" t="n">
-        <v>-14.91</v>
-      </c>
-      <c r="L42" s="3" t="n">
-        <v>11.83</v>
-      </c>
-      <c r="M42" s="3" t="n">
-        <v>-61.94</v>
-      </c>
-      <c r="N42" s="3" t="n">
-        <v>6.36</v>
-      </c>
-      <c r="O42" s="3" t="n">
-        <v>26.04</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>17</v>
+      <c r="J42" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>0</v>
@@ -2470,26 +1698,8 @@
       <c r="I43" s="3" t="n">
         <v>-4.04</v>
       </c>
-      <c r="J43" s="3" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="K43" s="3" t="n">
-        <v>-12.1</v>
-      </c>
-      <c r="L43" s="3" t="n">
-        <v>8.88</v>
-      </c>
-      <c r="M43" s="3" t="n">
-        <v>-55.56</v>
-      </c>
-      <c r="N43" s="3" t="n">
-        <v>22.37</v>
-      </c>
-      <c r="O43" s="3" t="n">
-        <v>29.77</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>17</v>
+      <c r="J43" s="4" t="n">
+        <v>-62.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>